<commit_message>
JOSN and loot tables and scripts finalized
</commit_message>
<xml_diff>
--- a/data/hg/loot_tables/minecraft_loot.xlsx
+++ b/data/hg/loot_tables/minecraft_loot.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chrome\curseforge\minecraft\Instances\Skullex's Zombie Horde 2\saves\Mosslorn V1.4\datapacks\ZombieHorde\data\hg\loot_tables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0F1B8F-38D6-42E2-99C7-35B6ED95FD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="4575" yWindow="720" windowWidth="21600" windowHeight="11835" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="pool1" sheetId="1" r:id="rId1"/>
+    <sheet name="pool2" sheetId="2" r:id="rId2"/>
+    <sheet name="pool2.1" sheetId="3" r:id="rId3"/>
+    <sheet name="pool2.2" sheetId="4" r:id="rId4"/>
+    <sheet name="pool2.3" sheetId="5" r:id="rId5"/>
+    <sheet name="pool3" sheetId="6" r:id="rId6"/>
+    <sheet name="pool3.1" sheetId="7" r:id="rId7"/>
+    <sheet name="pool3.2" sheetId="8" r:id="rId8"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="194">
   <si>
     <t>gun</t>
   </si>
@@ -227,35 +243,464 @@
   </si>
   <si>
     <t>win_30-30</t>
+  </si>
+  <si>
+    <t>light_grenade</t>
+  </si>
+  <si>
+    <t>baseball_grenade</t>
+  </si>
+  <si>
+    <t>coyote_sight</t>
+  </si>
+  <si>
+    <t>aimpoint_t2</t>
+  </si>
+  <si>
+    <t>aimpoint_t1</t>
+  </si>
+  <si>
+    <t>eotech_n</t>
+  </si>
+  <si>
+    <t>vortex_uh_1</t>
+  </si>
+  <si>
+    <t>eotech_short</t>
+  </si>
+  <si>
+    <t>srs_red_dot</t>
+  </si>
+  <si>
+    <t>acog_4x_scope</t>
+  </si>
+  <si>
+    <t>qmk152</t>
+  </si>
+  <si>
+    <t>elcan_14x</t>
+  </si>
+  <si>
+    <t>mini_dot</t>
+  </si>
+  <si>
+    <t>sro_dot</t>
+  </si>
+  <si>
+    <t>lpvo_1_6</t>
+  </si>
+  <si>
+    <t>8x_scope</t>
+  </si>
+  <si>
+    <t>grenade</t>
+  </si>
+  <si>
+    <t>attachment</t>
+  </si>
+  <si>
+    <t>pistol_silencer</t>
+  </si>
+  <si>
+    <t>small_extended_mag</t>
+  </si>
+  <si>
+    <t>light_stock</t>
+  </si>
+  <si>
+    <t>muzzle_brake</t>
+  </si>
+  <si>
+    <t>basic_laser</t>
+  </si>
+  <si>
+    <t>light_grip</t>
+  </si>
+  <si>
+    <t>weighted_stock</t>
+  </si>
+  <si>
+    <t>medium_extended_mag</t>
+  </si>
+  <si>
+    <t>tactical_stock</t>
+  </si>
+  <si>
+    <t>specialised_grip</t>
+  </si>
+  <si>
+    <t>Silencer</t>
+  </si>
+  <si>
+    <t>muzzle_compensator</t>
+  </si>
+  <si>
+    <t>large_extended_mag</t>
+  </si>
+  <si>
+    <t>ir_laser</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>broken_bottle</t>
+  </si>
+  <si>
+    <t>baseball_bat</t>
+  </si>
+  <si>
+    <t>night_stick</t>
+  </si>
+  <si>
+    <t>pipe</t>
+  </si>
+  <si>
+    <t>fire_extinguisher</t>
+  </si>
+  <si>
+    <t>tennis_racket</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>spiked_baseball_bat</t>
+  </si>
+  <si>
+    <t>spiked_plank</t>
+  </si>
+  <si>
+    <t>golf_stick</t>
+  </si>
+  <si>
+    <t>soap_in_a_sock</t>
+  </si>
+  <si>
+    <t>cleaver</t>
+  </si>
+  <si>
+    <t>guitar</t>
+  </si>
+  <si>
+    <t>red_crowbar</t>
+  </si>
+  <si>
+    <t>pipe_wrench</t>
+  </si>
+  <si>
+    <t>emergency_axe</t>
+  </si>
+  <si>
+    <t>fire_axe</t>
+  </si>
+  <si>
+    <t>head_cutter</t>
+  </si>
+  <si>
+    <t>katana</t>
+  </si>
+  <si>
+    <t>comically_large_spoon</t>
+  </si>
+  <si>
+    <t>red_football_armor_helmet</t>
+  </si>
+  <si>
+    <t>red_football_armor_chestplate</t>
+  </si>
+  <si>
+    <t>red_football_armor_leggings</t>
+  </si>
+  <si>
+    <t>red_football_armor_boots</t>
+  </si>
+  <si>
+    <t>blue_football_armor_helmet</t>
+  </si>
+  <si>
+    <t>blue_football_armor_chestplate</t>
+  </si>
+  <si>
+    <t>blue_football_armor_leggings</t>
+  </si>
+  <si>
+    <t>blue_football_armor_boots</t>
+  </si>
+  <si>
+    <t>ghilliesuit_helmet</t>
+  </si>
+  <si>
+    <t>ghilliesuit_chestplate</t>
+  </si>
+  <si>
+    <t>ghilliesuit_leggings</t>
+  </si>
+  <si>
+    <t>ghilliesuit_boots</t>
+  </si>
+  <si>
+    <t>sack_helmet</t>
+  </si>
+  <si>
+    <t>sheriff_helmet</t>
+  </si>
+  <si>
+    <t>hunting_chestplate</t>
+  </si>
+  <si>
+    <t>high_visibility_jacket_chestplate</t>
+  </si>
+  <si>
+    <t>balaclava_helmet</t>
+  </si>
+  <si>
+    <t>pink_balaclava_helmet</t>
+  </si>
+  <si>
+    <t>red_bikers_helmet</t>
+  </si>
+  <si>
+    <t>baseball_helmet_helmet</t>
+  </si>
+  <si>
+    <t>un_armor_helmet</t>
+  </si>
+  <si>
+    <t>hunting_helmet</t>
+  </si>
+  <si>
+    <t>fire_fighter_helmet</t>
+  </si>
+  <si>
+    <t>fire_fighter_chestplate</t>
+  </si>
+  <si>
+    <t>fire_fighter_leggings</t>
+  </si>
+  <si>
+    <t>fire_fighter_boots</t>
+  </si>
+  <si>
+    <t>police_helmet</t>
+  </si>
+  <si>
+    <t>police_chestplate</t>
+  </si>
+  <si>
+    <t>police_leggings</t>
+  </si>
+  <si>
+    <t>police_boots</t>
+  </si>
+  <si>
+    <t>grenade_belt_chestplate</t>
+  </si>
+  <si>
+    <t>press_bulletproof_vest_chestplate</t>
+  </si>
+  <si>
+    <t>swatriotcontrol_helmet</t>
+  </si>
+  <si>
+    <t>swatriotcontrol_chestplate</t>
+  </si>
+  <si>
+    <t>swatriotcontrol_leggings</t>
+  </si>
+  <si>
+    <t>swatriotcontrol_boots</t>
+  </si>
+  <si>
+    <t>red_motorcycle_helmet_helmet</t>
+  </si>
+  <si>
+    <t>black_motorcycle_helmet_helmet</t>
+  </si>
+  <si>
+    <t>spec_ops_helmet</t>
+  </si>
+  <si>
+    <t>spec_ops_chestplate</t>
+  </si>
+  <si>
+    <t>spec_ops_leggings</t>
+  </si>
+  <si>
+    <t>spec_ops_boots</t>
+  </si>
+  <si>
+    <t>welding_mask_helmet</t>
+  </si>
+  <si>
+    <t>dead_cockroach</t>
+  </si>
+  <si>
+    <t>chips</t>
+  </si>
+  <si>
+    <t>coke</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>vodka</t>
+  </si>
+  <si>
+    <t>whisky</t>
+  </si>
+  <si>
+    <t>hamburger</t>
+  </si>
+  <si>
+    <t>chocolate_bar</t>
+  </si>
+  <si>
+    <t>can_opener</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>canned_beans</t>
+  </si>
+  <si>
+    <t>canned_soup</t>
+  </si>
+  <si>
+    <t>canned_corn</t>
+  </si>
+  <si>
+    <t>canned_fish</t>
+  </si>
+  <si>
+    <t>energy_drink</t>
+  </si>
+  <si>
+    <t>canteen_44</t>
+  </si>
+  <si>
+    <t>mre</t>
+  </si>
+  <si>
+    <t>medicalkit</t>
+  </si>
+  <si>
+    <t>adrenaline_syringe</t>
+  </si>
+  <si>
+    <t>morphine</t>
+  </si>
+  <si>
+    <t>cocktail_molotov_green</t>
+  </si>
+  <si>
+    <t>armor</t>
+  </si>
+  <si>
+    <t>consumable</t>
+  </si>
+  <si>
+    <t>melee</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF356854"/>
+        <bgColor rgb="FF356854"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF34A853"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A86E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4285F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF674EA7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA4335"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="13">
-    <border/>
+  <borders count="14">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF284E3F"/>
@@ -269,6 +714,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -283,6 +729,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -297,6 +744,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -311,6 +759,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -325,6 +774,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -339,6 +789,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -353,6 +804,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -367,6 +819,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -381,6 +834,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -395,6 +849,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -409,6 +864,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -423,121 +879,169 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="28">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F9FA"/>
+          <bgColor rgb="FFF8F9FA"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF356854"/>
           <bgColor rgb="FF356854"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F9FA"/>
-          <bgColor rgb="FFF8F9FA"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Sheet1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C54" displayName="Table1" name="Table1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C54">
   <tableColumns count="3">
-    <tableColumn name="gun" id="1"/>
-    <tableColumn name="ammo" id="2"/>
-    <tableColumn name="rarity" id="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="gun"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ammo"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="rarity"/>
   </tableColumns>
-  <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -727,26 +1231,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="13.5"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -757,7 +1264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -765,10 +1272,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -776,10 +1283,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="9">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -787,10 +1294,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="6">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -798,10 +1305,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="9">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -809,10 +1316,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="6">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -820,10 +1327,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="9">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -831,10 +1338,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="6">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -842,10 +1349,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -853,10 +1360,10 @@
         <v>16</v>
       </c>
       <c r="C10" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -864,10 +1371,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="9">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -875,10 +1382,10 @@
         <v>16</v>
       </c>
       <c r="C12" s="6">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -886,10 +1393,10 @@
         <v>16</v>
       </c>
       <c r="C13" s="9">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -897,10 +1404,10 @@
         <v>16</v>
       </c>
       <c r="C14" s="6">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
@@ -908,10 +1415,10 @@
         <v>22</v>
       </c>
       <c r="C15" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
@@ -919,10 +1426,10 @@
         <v>24</v>
       </c>
       <c r="C16" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
@@ -930,10 +1437,10 @@
         <v>24</v>
       </c>
       <c r="C17" s="9">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
@@ -941,10 +1448,10 @@
         <v>24</v>
       </c>
       <c r="C18" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>27</v>
       </c>
@@ -952,10 +1459,10 @@
         <v>24</v>
       </c>
       <c r="C19" s="9">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>28</v>
       </c>
@@ -963,10 +1470,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
@@ -974,10 +1481,10 @@
         <v>24</v>
       </c>
       <c r="C21" s="9">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
@@ -985,10 +1492,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="6">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>31</v>
       </c>
@@ -996,10 +1503,10 @@
         <v>24</v>
       </c>
       <c r="C23" s="9">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
@@ -1007,10 +1514,10 @@
         <v>24</v>
       </c>
       <c r="C24" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>33</v>
       </c>
@@ -1018,10 +1525,10 @@
         <v>24</v>
       </c>
       <c r="C25" s="9">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1029,10 +1536,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>35</v>
       </c>
@@ -1040,10 +1547,10 @@
         <v>24</v>
       </c>
       <c r="C27" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
@@ -1051,10 +1558,10 @@
         <v>37</v>
       </c>
       <c r="C28" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>38</v>
       </c>
@@ -1062,10 +1569,10 @@
         <v>37</v>
       </c>
       <c r="C29" s="9">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>39</v>
       </c>
@@ -1073,10 +1580,10 @@
         <v>40</v>
       </c>
       <c r="C30" s="6">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>41</v>
       </c>
@@ -1084,10 +1591,10 @@
         <v>42</v>
       </c>
       <c r="C31" s="9">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>43</v>
       </c>
@@ -1095,10 +1602,10 @@
         <v>42</v>
       </c>
       <c r="C32" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>44</v>
       </c>
@@ -1106,10 +1613,10 @@
         <v>42</v>
       </c>
       <c r="C33" s="9">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>45</v>
       </c>
@@ -1117,10 +1624,10 @@
         <v>42</v>
       </c>
       <c r="C34" s="6">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>46</v>
       </c>
@@ -1128,10 +1635,10 @@
         <v>42</v>
       </c>
       <c r="C35" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>47</v>
       </c>
@@ -1139,10 +1646,10 @@
         <v>42</v>
       </c>
       <c r="C36" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>48</v>
       </c>
@@ -1150,10 +1657,10 @@
         <v>49</v>
       </c>
       <c r="C37" s="9">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>50</v>
       </c>
@@ -1161,10 +1668,10 @@
         <v>51</v>
       </c>
       <c r="C38" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>52</v>
       </c>
@@ -1172,10 +1679,10 @@
         <v>51</v>
       </c>
       <c r="C39" s="9">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
@@ -1183,10 +1690,10 @@
         <v>54</v>
       </c>
       <c r="C40" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>55</v>
       </c>
@@ -1194,10 +1701,10 @@
         <v>54</v>
       </c>
       <c r="C41" s="9">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>56</v>
       </c>
@@ -1205,10 +1712,10 @@
         <v>54</v>
       </c>
       <c r="C42" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>57</v>
       </c>
@@ -1216,10 +1723,10 @@
         <v>54</v>
       </c>
       <c r="C43" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>58</v>
       </c>
@@ -1227,10 +1734,10 @@
         <v>54</v>
       </c>
       <c r="C44" s="6">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>59</v>
       </c>
@@ -1238,10 +1745,10 @@
         <v>54</v>
       </c>
       <c r="C45" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>60</v>
       </c>
@@ -1249,10 +1756,10 @@
         <v>54</v>
       </c>
       <c r="C46" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>61</v>
       </c>
@@ -1260,10 +1767,10 @@
         <v>62</v>
       </c>
       <c r="C47" s="9">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>63</v>
       </c>
@@ -1271,10 +1778,10 @@
         <v>62</v>
       </c>
       <c r="C48" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>64</v>
       </c>
@@ -1282,10 +1789,10 @@
         <v>62</v>
       </c>
       <c r="C49" s="9">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>65</v>
       </c>
@@ -1293,10 +1800,10 @@
         <v>62</v>
       </c>
       <c r="C50" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>66</v>
       </c>
@@ -1304,10 +1811,10 @@
         <v>62</v>
       </c>
       <c r="C51" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>67</v>
       </c>
@@ -1315,10 +1822,10 @@
         <v>62</v>
       </c>
       <c r="C52" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>68</v>
       </c>
@@ -1326,10 +1833,10 @@
         <v>69</v>
       </c>
       <c r="C53" s="9">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>70</v>
       </c>
@@ -1337,19 +1844,1308 @@
         <v>71</v>
       </c>
       <c r="C54" s="12">
-        <v>3.0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C54">
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C54" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>AND(ISNUMBER(C2),(NOT(OR(NOT(ISERROR(DATEVALUE(C2))), AND(ISNUMBER(C2), LEFT(CELL("format", C2))="D")))))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:B54"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:B54" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E966D093-77BB-455F-AFB1-C3BD028875F2}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:B54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06519182-227B-484D-B2F6-9BFB9EFA6C87}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C810A878-DD45-40ED-ABE8-1D72BFB0AC4D}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03CE4E2A-B4EA-4C4D-89C0-4AB63627D219}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABECAD1-4348-4A26-9784-61A5349A624F}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A1A7A2-6EF8-4EF3-B110-85D353CA7B7F}">
+  <dimension ref="A1:B44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687EA104-781E-4A9C-ABBD-368F0629E2C5}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>